<commit_message>
Curate substrate usage EXCEL file
</commit_message>
<xml_diff>
--- a/Basic assessment/M_yeastGEM_v8__46__3__46__0_sub_use.xlsx
+++ b/Basic assessment/M_yeastGEM_v8__46__3__46__0_sub_use.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\model_research\yeast_GEM_multi_omics_analysis\Figure2a_2b\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\model_research\yeast_GEM_multi_omics_analysis\Basic assessment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92F768A5-2618-46DE-BE2D-8F22365823DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AFE626-ABF9-4498-9062-A7B43A460947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5490" yWindow="2115" windowWidth="18810" windowHeight="13530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,9 +571,6 @@
     <t>s_4150[e]</t>
   </si>
   <si>
-    <t>s_4156[e]</t>
-  </si>
-  <si>
     <t>s_0576[e]</t>
   </si>
   <si>
@@ -956,6 +953,10 @@
   </si>
   <si>
     <t>NG</t>
+  </si>
+  <si>
+    <t>s_0572[c]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1334,7 +1335,7 @@
   <dimension ref="A1:F185"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1370,13 +1371,13 @@
         <v>155</v>
       </c>
       <c r="D2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.15">
@@ -1390,13 +1391,13 @@
         <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.15">
@@ -1410,13 +1411,13 @@
         <v>157</v>
       </c>
       <c r="D4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.15">
@@ -1430,13 +1431,13 @@
         <v>158</v>
       </c>
       <c r="D5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F5" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.15">
@@ -1450,13 +1451,13 @@
         <v>159</v>
       </c>
       <c r="D6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.15">
@@ -1470,13 +1471,13 @@
         <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1490,13 +1491,13 @@
         <v>161</v>
       </c>
       <c r="D8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1510,13 +1511,13 @@
         <v>162</v>
       </c>
       <c r="D9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.15">
@@ -1530,13 +1531,13 @@
         <v>163</v>
       </c>
       <c r="D10" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1550,13 +1551,13 @@
         <v>164</v>
       </c>
       <c r="D11" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F11" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1570,13 +1571,13 @@
         <v>165</v>
       </c>
       <c r="D12" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F12" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.15">
@@ -1590,13 +1591,13 @@
         <v>166</v>
       </c>
       <c r="D13" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1610,13 +1611,13 @@
         <v>167</v>
       </c>
       <c r="D14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E14" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.15">
@@ -1630,13 +1631,13 @@
         <v>168</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1650,13 +1651,13 @@
         <v>168</v>
       </c>
       <c r="D16" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F16" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1670,13 +1671,13 @@
         <v>169</v>
       </c>
       <c r="D17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F17" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1690,13 +1691,13 @@
         <v>170</v>
       </c>
       <c r="D18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F18" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1710,13 +1711,13 @@
         <v>171</v>
       </c>
       <c r="D19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
@@ -1730,13 +1731,13 @@
         <v>172</v>
       </c>
       <c r="D20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1750,13 +1751,13 @@
         <v>173</v>
       </c>
       <c r="D21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F21" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1770,13 +1771,13 @@
         <v>174</v>
       </c>
       <c r="D22" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E22" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F22" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -1790,13 +1791,13 @@
         <v>175</v>
       </c>
       <c r="D23" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F23" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.15">
@@ -1810,13 +1811,13 @@
         <v>176</v>
       </c>
       <c r="D24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.15">
@@ -1830,13 +1831,13 @@
         <v>177</v>
       </c>
       <c r="D25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F25" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">
@@ -1850,13 +1851,13 @@
         <v>178</v>
       </c>
       <c r="D26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F26" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.15">
@@ -1870,13 +1871,13 @@
         <v>179</v>
       </c>
       <c r="D27" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E27" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F27" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.15">
@@ -1890,13 +1891,13 @@
         <v>180</v>
       </c>
       <c r="D28" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E28" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F28" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.15">
@@ -1910,13 +1911,13 @@
         <v>181</v>
       </c>
       <c r="D29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.15">
@@ -1927,16 +1928,16 @@
         <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>182</v>
+        <v>310</v>
       </c>
       <c r="D30" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.15">
@@ -1947,16 +1948,16 @@
         <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D31" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F31" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.15">
@@ -1967,16 +1968,16 @@
         <v>34</v>
       </c>
       <c r="C32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D32" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.15">
@@ -1987,16 +1988,16 @@
         <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D33" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E33" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F33" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2007,16 +2008,16 @@
         <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D34" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F34" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.15">
@@ -2027,16 +2028,16 @@
         <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D35" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F35" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.15">
@@ -2047,16 +2048,16 @@
         <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E36" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2067,16 +2068,16 @@
         <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D37" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E37" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F37" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.15">
@@ -2087,16 +2088,16 @@
         <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D38" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E38" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F38" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.15">
@@ -2107,16 +2108,16 @@
         <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F39" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.15">
@@ -2127,16 +2128,16 @@
         <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D40" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E40" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2147,16 +2148,16 @@
         <v>41</v>
       </c>
       <c r="C41" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2167,16 +2168,16 @@
         <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F42" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.15">
@@ -2187,16 +2188,16 @@
         <v>43</v>
       </c>
       <c r="C43" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D43" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.15">
@@ -2207,16 +2208,16 @@
         <v>44</v>
       </c>
       <c r="C44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D44" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F44" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.15">
@@ -2227,16 +2228,16 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D45" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E45" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F45" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.15">
@@ -2247,16 +2248,16 @@
         <v>46</v>
       </c>
       <c r="C46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D46" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E46" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F46" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2267,16 +2268,16 @@
         <v>47</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D47" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F47" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2287,16 +2288,16 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D48" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E48" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F48" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2307,16 +2308,16 @@
         <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D49" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F49" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.15">
@@ -2327,16 +2328,16 @@
         <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D50" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F50" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2347,16 +2348,16 @@
         <v>50</v>
       </c>
       <c r="C51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D51" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F51" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.15">
@@ -2367,16 +2368,16 @@
         <v>51</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D52" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E52" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F52" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.15">
@@ -2387,16 +2388,16 @@
         <v>52</v>
       </c>
       <c r="C53" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D53" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F53" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2407,16 +2408,16 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D54" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F54" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.15">
@@ -2427,16 +2428,16 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D55" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E55" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F55" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.15">
@@ -2447,16 +2448,16 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D56" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E56" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F56" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.15">
@@ -2467,16 +2468,16 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E57" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F57" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2487,16 +2488,16 @@
         <v>55</v>
       </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D58" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E58" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F58" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.15">
@@ -2507,16 +2508,16 @@
         <v>56</v>
       </c>
       <c r="C59" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D59" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E59" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F59" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2527,16 +2528,16 @@
         <v>56</v>
       </c>
       <c r="C60" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D60" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F60" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.15">
@@ -2547,16 +2548,16 @@
         <v>57</v>
       </c>
       <c r="C61" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D61" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E61" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F61" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2567,16 +2568,16 @@
         <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F62" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2587,16 +2588,16 @@
         <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F63" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2607,16 +2608,16 @@
         <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D64" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E64" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F64" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2627,16 +2628,16 @@
         <v>59</v>
       </c>
       <c r="C65" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D65" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E65" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2647,13 +2648,13 @@
         <v>60</v>
       </c>
       <c r="C66" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D66" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E66" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.15">
@@ -2664,16 +2665,16 @@
         <v>61</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D67" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E67" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F67" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2684,16 +2685,16 @@
         <v>61</v>
       </c>
       <c r="C68" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D68" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.15">
@@ -2704,16 +2705,16 @@
         <v>62</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D69" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E69" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F69" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2724,16 +2725,16 @@
         <v>62</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D70" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E70" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F70" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.15">
@@ -2744,16 +2745,16 @@
         <v>63</v>
       </c>
       <c r="C71" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D71" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E71" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F71" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2764,16 +2765,16 @@
         <v>63</v>
       </c>
       <c r="C72" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D72" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E72" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F72" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.15">
@@ -2784,16 +2785,16 @@
         <v>64</v>
       </c>
       <c r="C73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D73" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E73" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2804,16 +2805,16 @@
         <v>64</v>
       </c>
       <c r="C74" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D74" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E74" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F74" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.15">
@@ -2824,16 +2825,16 @@
         <v>65</v>
       </c>
       <c r="C75" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D75" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E75" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F75" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2844,16 +2845,16 @@
         <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.15">
@@ -2864,16 +2865,16 @@
         <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D77" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E77" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F77" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2884,16 +2885,16 @@
         <v>66</v>
       </c>
       <c r="C78" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D78" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E78" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F78" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.15">
@@ -2904,16 +2905,16 @@
         <v>67</v>
       </c>
       <c r="C79" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F79" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2924,16 +2925,16 @@
         <v>67</v>
       </c>
       <c r="C80" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D80" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F80" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.15">
@@ -2944,16 +2945,16 @@
         <v>68</v>
       </c>
       <c r="C81" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D81" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E81" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F81" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -2964,16 +2965,16 @@
         <v>68</v>
       </c>
       <c r="C82" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D82" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E82" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F82" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.15">
@@ -2984,16 +2985,16 @@
         <v>69</v>
       </c>
       <c r="C83" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D83" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E83" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F83" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3004,16 +3005,16 @@
         <v>69</v>
       </c>
       <c r="C84" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D84" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F84" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3024,16 +3025,16 @@
         <v>69</v>
       </c>
       <c r="C85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E85" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F85" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.15">
@@ -3044,16 +3045,16 @@
         <v>70</v>
       </c>
       <c r="C86" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D86" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E86" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F86" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3064,16 +3065,16 @@
         <v>70</v>
       </c>
       <c r="C87" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D87" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E87" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F87" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.15">
@@ -3084,16 +3085,16 @@
         <v>71</v>
       </c>
       <c r="C88" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D88" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E88" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F88" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3104,16 +3105,16 @@
         <v>71</v>
       </c>
       <c r="C89" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D89" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E89" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F89" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.15">
@@ -3124,16 +3125,16 @@
         <v>72</v>
       </c>
       <c r="C90" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D90" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E90" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F90" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3144,16 +3145,16 @@
         <v>72</v>
       </c>
       <c r="C91" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D91" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F91" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.15">
@@ -3164,16 +3165,16 @@
         <v>73</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D92" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E92" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F92" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.15">
@@ -3184,16 +3185,16 @@
         <v>74</v>
       </c>
       <c r="C93" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D93" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E93" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F93" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3204,16 +3205,16 @@
         <v>74</v>
       </c>
       <c r="C94" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D94" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E94" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F94" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3224,16 +3225,16 @@
         <v>75</v>
       </c>
       <c r="C95" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D95" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E95" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F95" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3244,16 +3245,16 @@
         <v>76</v>
       </c>
       <c r="C96" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D96" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E96" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F96" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.15">
@@ -3264,16 +3265,16 @@
         <v>77</v>
       </c>
       <c r="C97" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D97" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E97" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F97" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3284,16 +3285,16 @@
         <v>77</v>
       </c>
       <c r="C98" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D98" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E98" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F98" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3304,13 +3305,13 @@
         <v>78</v>
       </c>
       <c r="C99" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D99" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E99" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.15">
@@ -3321,16 +3322,16 @@
         <v>79</v>
       </c>
       <c r="C100" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D100" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E100" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F100" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.15">
@@ -3341,16 +3342,16 @@
         <v>80</v>
       </c>
       <c r="C101" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D101" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E101" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F101" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.15">
@@ -3361,16 +3362,16 @@
         <v>81</v>
       </c>
       <c r="C102" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D102" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E102" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F102" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.15">
@@ -3381,16 +3382,16 @@
         <v>82</v>
       </c>
       <c r="C103" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D103" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E103" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F103" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3401,16 +3402,16 @@
         <v>82</v>
       </c>
       <c r="C104" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E104" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F104" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3421,16 +3422,16 @@
         <v>83</v>
       </c>
       <c r="C105" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D105" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E105" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F105" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3441,16 +3442,16 @@
         <v>84</v>
       </c>
       <c r="C106" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D106" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F106" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.15">
@@ -3461,16 +3462,16 @@
         <v>85</v>
       </c>
       <c r="C107" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D107" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E107" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F107" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3481,16 +3482,16 @@
         <v>86</v>
       </c>
       <c r="C108" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D108" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E108" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F108" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3501,16 +3502,16 @@
         <v>87</v>
       </c>
       <c r="C109" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D109" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E109" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F109" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.15">
@@ -3521,16 +3522,16 @@
         <v>88</v>
       </c>
       <c r="C110" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D110" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E110" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F110" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3541,16 +3542,16 @@
         <v>88</v>
       </c>
       <c r="C111" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D111" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E111" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F111" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.15">
@@ -3561,16 +3562,16 @@
         <v>89</v>
       </c>
       <c r="C112" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D112" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E112" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F112" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.15">
@@ -3581,16 +3582,16 @@
         <v>90</v>
       </c>
       <c r="C113" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D113" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E113" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F113" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.15">
@@ -3601,16 +3602,16 @@
         <v>91</v>
       </c>
       <c r="C114" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D114" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E114" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F114" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3621,16 +3622,16 @@
         <v>92</v>
       </c>
       <c r="C115" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D115" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E115" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F115" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.15">
@@ -3641,16 +3642,16 @@
         <v>93</v>
       </c>
       <c r="C116" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D116" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E116" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F116" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3661,16 +3662,16 @@
         <v>93</v>
       </c>
       <c r="C117" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D117" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E117" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F117" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.15">
@@ -3681,16 +3682,16 @@
         <v>94</v>
       </c>
       <c r="C118" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D118" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E118" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F118" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3701,16 +3702,16 @@
         <v>95</v>
       </c>
       <c r="C119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D119" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F119" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3721,16 +3722,16 @@
         <v>96</v>
       </c>
       <c r="C120" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D120" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E120" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F120" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3741,16 +3742,16 @@
         <v>97</v>
       </c>
       <c r="C121" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D121" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F121" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.15">
@@ -3761,16 +3762,16 @@
         <v>98</v>
       </c>
       <c r="C122" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D122" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E122" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F122" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3781,16 +3782,16 @@
         <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D123" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E123" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F123" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3801,16 +3802,16 @@
         <v>99</v>
       </c>
       <c r="C124" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D124" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.15">
@@ -3821,16 +3822,16 @@
         <v>100</v>
       </c>
       <c r="C125" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D125" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E125" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F125" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.15">
@@ -3841,16 +3842,16 @@
         <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D126" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E126" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F126" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.15">
@@ -3861,16 +3862,16 @@
         <v>102</v>
       </c>
       <c r="C127" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D127" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E127" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F127" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.15">
@@ -3881,16 +3882,16 @@
         <v>103</v>
       </c>
       <c r="C128" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D128" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E128" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F128" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.15">
@@ -3901,16 +3902,16 @@
         <v>104</v>
       </c>
       <c r="C129" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D129" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E129" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F129" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.15">
@@ -3921,16 +3922,16 @@
         <v>105</v>
       </c>
       <c r="C130" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D130" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E130" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F130" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -3941,16 +3942,16 @@
         <v>106</v>
       </c>
       <c r="C131" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D131" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E131" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F131" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.15">
@@ -3961,16 +3962,16 @@
         <v>107</v>
       </c>
       <c r="C132" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D132" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E132" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F132" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.15">
@@ -3981,16 +3982,16 @@
         <v>108</v>
       </c>
       <c r="C133" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D133" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E133" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F133" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.15">
@@ -4001,16 +4002,16 @@
         <v>109</v>
       </c>
       <c r="C134" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D134" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E134" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F134" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4021,16 +4022,16 @@
         <v>109</v>
       </c>
       <c r="C135" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D135" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E135" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F135" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.15">
@@ -4041,16 +4042,16 @@
         <v>110</v>
       </c>
       <c r="C136" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D136" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E136" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F136" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4061,16 +4062,16 @@
         <v>110</v>
       </c>
       <c r="C137" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D137" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E137" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F137" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4081,16 +4082,16 @@
         <v>111</v>
       </c>
       <c r="C138" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D138" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E138" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F138" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.15">
@@ -4101,16 +4102,16 @@
         <v>112</v>
       </c>
       <c r="C139" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D139" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E139" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F139" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.15">
@@ -4121,16 +4122,16 @@
         <v>113</v>
       </c>
       <c r="C140" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D140" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E140" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F140" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4141,16 +4142,16 @@
         <v>113</v>
       </c>
       <c r="C141" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D141" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E141" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F141" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4161,16 +4162,16 @@
         <v>114</v>
       </c>
       <c r="C142" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D142" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E142" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F142" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4181,16 +4182,16 @@
         <v>115</v>
       </c>
       <c r="C143" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D143" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E143" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F143" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.15">
@@ -4201,16 +4202,16 @@
         <v>116</v>
       </c>
       <c r="C144" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D144" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4221,16 +4222,16 @@
         <v>116</v>
       </c>
       <c r="C145" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D145" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E145" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F145" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.15">
@@ -4241,16 +4242,16 @@
         <v>117</v>
       </c>
       <c r="C146" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D146" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E146" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F146" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.15">
@@ -4261,16 +4262,16 @@
         <v>118</v>
       </c>
       <c r="C147" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D147" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E147" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F147" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.15">
@@ -4281,16 +4282,16 @@
         <v>119</v>
       </c>
       <c r="C148" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D148" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E148" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F148" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4301,13 +4302,13 @@
         <v>120</v>
       </c>
       <c r="C149" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D149" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E149" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.15">
@@ -4318,16 +4319,16 @@
         <v>121</v>
       </c>
       <c r="C150" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D150" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E150" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F150" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4338,16 +4339,16 @@
         <v>121</v>
       </c>
       <c r="C151" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D151" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E151" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="F151" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4358,16 +4359,16 @@
         <v>122</v>
       </c>
       <c r="C152" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D152" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E152" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F152" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4378,16 +4379,16 @@
         <v>123</v>
       </c>
       <c r="C153" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D153" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E153" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F153" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4398,16 +4399,16 @@
         <v>124</v>
       </c>
       <c r="C154" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D154" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E154" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F154" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4418,16 +4419,16 @@
         <v>125</v>
       </c>
       <c r="C155" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D155" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E155" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F155" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4438,16 +4439,16 @@
         <v>126</v>
       </c>
       <c r="C156" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D156" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E156" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F156" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4458,16 +4459,16 @@
         <v>127</v>
       </c>
       <c r="C157" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D157" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E157" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F157" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4478,16 +4479,16 @@
         <v>128</v>
       </c>
       <c r="C158" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D158" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E158" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F158" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4498,16 +4499,16 @@
         <v>129</v>
       </c>
       <c r="C159" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D159" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E159" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F159" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4518,16 +4519,16 @@
         <v>130</v>
       </c>
       <c r="C160" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D160" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E160" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F160" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4538,16 +4539,16 @@
         <v>131</v>
       </c>
       <c r="C161" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D161" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F161" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4558,16 +4559,16 @@
         <v>132</v>
       </c>
       <c r="C162" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D162" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E162" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F162" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4578,16 +4579,16 @@
         <v>133</v>
       </c>
       <c r="C163" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D163" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F163" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4598,16 +4599,16 @@
         <v>134</v>
       </c>
       <c r="C164" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D164" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E164" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F164" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4618,16 +4619,16 @@
         <v>135</v>
       </c>
       <c r="C165" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D165" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E165" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F165" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4638,16 +4639,16 @@
         <v>135</v>
       </c>
       <c r="C166" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D166" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E166" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F166" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4658,16 +4659,16 @@
         <v>136</v>
       </c>
       <c r="C167" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D167" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E167" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F167" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4678,16 +4679,16 @@
         <v>137</v>
       </c>
       <c r="C168" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D168" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E168" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F168" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4698,16 +4699,16 @@
         <v>138</v>
       </c>
       <c r="C169" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D169" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E169" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F169" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4718,16 +4719,16 @@
         <v>139</v>
       </c>
       <c r="C170" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D170" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E170" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F170" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4738,16 +4739,16 @@
         <v>140</v>
       </c>
       <c r="C171" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D171" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E171" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F171" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4758,16 +4759,16 @@
         <v>141</v>
       </c>
       <c r="C172" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D172" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E172" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F172" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.15">
@@ -4778,16 +4779,16 @@
         <v>142</v>
       </c>
       <c r="C173" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D173" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E173" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F173" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4798,16 +4799,16 @@
         <v>143</v>
       </c>
       <c r="C174" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D174" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E174" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F174" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4818,13 +4819,13 @@
         <v>144</v>
       </c>
       <c r="C175" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D175" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E175" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4835,16 +4836,16 @@
         <v>145</v>
       </c>
       <c r="C176" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D176" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E176" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F176" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="177" spans="1:6" x14ac:dyDescent="0.15">
@@ -4855,16 +4856,16 @@
         <v>146</v>
       </c>
       <c r="C177" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D177" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E177" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F177" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4875,16 +4876,16 @@
         <v>147</v>
       </c>
       <c r="C178" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D178" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E178" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F178" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.15">
@@ -4895,16 +4896,16 @@
         <v>148</v>
       </c>
       <c r="C179" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D179" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E179" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F179" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="180" spans="1:6" x14ac:dyDescent="0.15">
@@ -4915,16 +4916,16 @@
         <v>149</v>
       </c>
       <c r="C180" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D180" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E180" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F180" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.15">
@@ -4935,16 +4936,16 @@
         <v>150</v>
       </c>
       <c r="C181" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D181" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E181" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F181" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="182" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4955,16 +4956,16 @@
         <v>151</v>
       </c>
       <c r="C182" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D182" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E182" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F182" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.15">
@@ -4975,16 +4976,16 @@
         <v>152</v>
       </c>
       <c r="C183" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D183" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E183" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F183" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.15">
@@ -4995,16 +4996,16 @@
         <v>153</v>
       </c>
       <c r="C184" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D184" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E184" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F184" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.15">
@@ -5015,16 +5016,16 @@
         <v>154</v>
       </c>
       <c r="C185" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D185" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E185" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F185" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>